<commit_message>
fix copy/paste error in SPLASCHLiquidDietCS thin
</commit_message>
<xml_diff>
--- a/output/CodeSystem-SPLASCHLiquidDietCS.xlsx
+++ b/output/CodeSystem-SPLASCHLiquidDietCS.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-12-10T12:07:05-05:00</t>
+    <t>2021-12-10T13:11:15-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -144,7 +144,7 @@
     <t>thin</t>
   </si>
   <si>
-    <t>Regular</t>
+    <t>Thin</t>
   </si>
   <si>
     <t>slightly-thick</t>

</xml_diff>